<commit_message>
add credit rating from report, corporate website or agencies
</commit_message>
<xml_diff>
--- a/data/ticker_esg_data.xlsx
+++ b/data/ticker_esg_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="125">
   <si>
     <t>Company</t>
   </si>
@@ -37,48 +37,135 @@
     <t>moyenne paire</t>
   </si>
   <si>
+    <t>Moody's LT rating</t>
+  </si>
+  <si>
+    <t>Moody's ST rating</t>
+  </si>
+  <si>
+    <t>Moody's outlook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SnP LT rating </t>
+  </si>
+  <si>
+    <t>Snp ST rating</t>
+  </si>
+  <si>
+    <t>Snp outlook</t>
+  </si>
+  <si>
     <t>ArcelorMittal</t>
   </si>
   <si>
     <t>MT</t>
   </si>
   <si>
+    <t>Baa3</t>
+  </si>
+  <si>
+    <t>P-3</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>BBB-</t>
+  </si>
+  <si>
+    <t>A-3</t>
+  </si>
+  <si>
     <t>Airbus SAS</t>
   </si>
   <si>
     <t>AIR</t>
   </si>
   <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>P-1</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A-1</t>
+  </si>
+  <si>
     <t>Safran</t>
   </si>
   <si>
     <t>SAF.PA</t>
   </si>
   <si>
+    <t>A-</t>
+  </si>
+  <si>
     <t>Danone</t>
   </si>
   <si>
     <t>BN</t>
   </si>
   <si>
+    <t>Baa1</t>
+  </si>
+  <si>
+    <t>BBB+</t>
+  </si>
+  <si>
+    <t>A-2</t>
+  </si>
+  <si>
     <t>AXA</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>A-1+</t>
+  </si>
+  <si>
     <t>Renault</t>
   </si>
   <si>
     <t>RNO.PA</t>
   </si>
   <si>
+    <t>Ba2</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>BB+</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>Stellantis</t>
   </si>
   <si>
     <t>STLAP.PA</t>
   </si>
   <si>
+    <t>Baa2</t>
+  </si>
+  <si>
+    <t>P-2</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
     <t>BNP Paribas</t>
   </si>
   <si>
@@ -91,6 +178,12 @@
     <t>ACA</t>
   </si>
   <si>
+    <t>Aa2</t>
+  </si>
+  <si>
+    <t>AA-</t>
+  </si>
+  <si>
     <t>Societe Generale</t>
   </si>
   <si>
@@ -109,18 +202,27 @@
     <t>DG</t>
   </si>
   <si>
+    <t>A3</t>
+  </si>
+  <si>
     <t>Bouygues</t>
   </si>
   <si>
     <t>EN</t>
   </si>
   <si>
+    <t>A4</t>
+  </si>
+  <si>
     <t>L'Oreal</t>
   </si>
   <si>
     <t>OR</t>
   </si>
   <si>
+    <t>AA</t>
+  </si>
+  <si>
     <t>Carrefour</t>
   </si>
   <si>
@@ -145,6 +247,9 @@
     <t>HO</t>
   </si>
   <si>
+    <t>Negative</t>
+  </si>
+  <si>
     <t>Air Liquide</t>
   </si>
   <si>
@@ -157,6 +262,9 @@
     <t>URW</t>
   </si>
   <si>
+    <t>NR</t>
+  </si>
+  <si>
     <t>Alstom</t>
   </si>
   <si>
@@ -239,6 +347,9 @@
   </si>
   <si>
     <t>CAP.PA</t>
+  </si>
+  <si>
+    <t>Positive</t>
   </si>
   <si>
     <t>Dassault Systèmes</t>
@@ -281,7 +392,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -292,31 +403,75 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FFDDDEDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDDDEDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDDDEDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFDDDEDD"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,32 +718,84 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="C4" s="1">
         <v>23.0</v>
@@ -608,13 +815,22 @@
       <c r="H4" s="1">
         <v>2.3</v>
       </c>
+      <c r="K4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>20.0</v>
@@ -634,13 +850,28 @@
       <c r="H5" s="1">
         <v>2.1</v>
       </c>
+      <c r="I5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1">
         <v>17.0</v>
@@ -660,13 +891,31 @@
       <c r="H6" s="1">
         <v>1.5</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
+        <v>40</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C7" s="1">
         <v>23.0</v>
@@ -686,47 +935,101 @@
       <c r="H7" s="1">
         <v>2.4</v>
       </c>
+      <c r="I7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>46</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="7">
+        <v>25.0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="E9" s="7">
+        <v>11.2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>12.6</v>
+      </c>
+      <c r="G9" s="7">
+        <v>3.0</v>
+      </c>
+      <c r="H9" s="7">
+        <v>2.2</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3">
-        <v>25.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="E9" s="3">
-        <v>11.2</v>
-      </c>
-      <c r="F9" s="3">
-        <v>12.6</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2.2</v>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1">
         <v>25.0</v>
@@ -746,13 +1049,31 @@
       <c r="H10" s="1">
         <v>2.2</v>
       </c>
+      <c r="I10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C11" s="1">
         <v>20.0</v>
@@ -772,39 +1093,63 @@
       <c r="H11" s="1">
         <v>2.2</v>
       </c>
+      <c r="I11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="3">
+        <v>60</v>
+      </c>
+      <c r="C12" s="7">
         <v>17.0</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="7">
         <v>1.5</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="7">
         <v>9.8</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="7">
         <v>5.6</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="7">
         <v>1.0</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="7">
         <v>1.4</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1">
         <v>27.0</v>
@@ -824,13 +1169,31 @@
       <c r="H13" s="1">
         <v>2.3</v>
       </c>
+      <c r="I13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1">
         <v>36.0</v>
@@ -850,13 +1213,31 @@
       <c r="H14" s="1">
         <v>2.1</v>
       </c>
+      <c r="I14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1">
         <v>17.0</v>
@@ -876,13 +1257,28 @@
       <c r="H15" s="1">
         <v>1.8</v>
       </c>
+      <c r="I15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="C16" s="1">
         <v>23.0</v>
@@ -902,13 +1298,28 @@
       <c r="H16" s="1">
         <v>2.0</v>
       </c>
+      <c r="I16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>72</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="C17" s="1">
         <v>29.0</v>
@@ -928,13 +1339,31 @@
       <c r="H17" s="1">
         <v>1.8</v>
       </c>
+      <c r="I17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1">
         <v>21.0</v>
@@ -954,13 +1383,31 @@
       <c r="H18" s="1">
         <v>1.6</v>
       </c>
+      <c r="I18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C19" s="1">
         <v>29.0</v>
@@ -980,13 +1427,28 @@
       <c r="H19" s="1">
         <v>2.1</v>
       </c>
+      <c r="I19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C20" s="1">
         <v>14.0</v>
@@ -1006,13 +1468,31 @@
       <c r="H20" s="1">
         <v>1.5</v>
       </c>
+      <c r="I20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="C21" s="1">
         <v>5.0</v>
@@ -1032,13 +1512,31 @@
       <c r="H21" s="1">
         <v>0.6</v>
       </c>
+      <c r="I21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1">
         <v>19.0</v>
@@ -1058,47 +1556,86 @@
       <c r="H22" s="1">
         <v>1.4</v>
       </c>
+      <c r="I22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="3">
+        <v>88</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="7">
         <v>12.0</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="7">
         <v>0.8</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="7">
         <v>5.9</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="7">
         <v>5.7</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="7">
         <v>2.0</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="7">
         <v>1.8</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>90</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="C25" s="1">
         <v>10.0</v>
@@ -1121,10 +1658,10 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>92</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="C26" s="1">
         <v>11.0</v>
@@ -1144,13 +1681,22 @@
       <c r="H26" s="1">
         <v>1.8</v>
       </c>
+      <c r="L26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="C27" s="1">
         <v>20.0</v>
@@ -1170,13 +1716,20 @@
       <c r="H27" s="1">
         <v>1.1</v>
       </c>
+      <c r="I27" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="C28" s="1">
         <v>17.0</v>
@@ -1196,13 +1749,28 @@
       <c r="H28" s="1">
         <v>1.5</v>
       </c>
+      <c r="I28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>98</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="C29" s="1">
         <v>15.0</v>
@@ -1222,13 +1790,28 @@
       <c r="H29" s="1">
         <v>1.5</v>
       </c>
+      <c r="I29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="C30" s="1">
         <v>11.0</v>
@@ -1248,13 +1831,19 @@
       <c r="H30" s="1">
         <v>1.4</v>
       </c>
+      <c r="I30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="C31" s="1">
         <v>20.0</v>
@@ -1274,13 +1863,31 @@
       <c r="H31" s="1">
         <v>1.6</v>
       </c>
+      <c r="I31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="C32" s="1">
         <v>22.0</v>
@@ -1300,13 +1907,31 @@
       <c r="H32" s="1">
         <v>1.9</v>
       </c>
+      <c r="I32" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>106</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="C33" s="1">
         <v>12.0</v>
@@ -1326,13 +1951,28 @@
       <c r="H33" s="1">
         <v>1.6</v>
       </c>
+      <c r="I33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="C34" s="1">
         <v>11.0</v>
@@ -1352,13 +1992,25 @@
       <c r="H34" s="1">
         <v>1.2</v>
       </c>
+      <c r="I34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>75</v>
+        <v>110</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="C35" s="1">
         <v>10.0</v>
@@ -1378,13 +2030,19 @@
       <c r="H35" s="1">
         <v>1.2</v>
       </c>
+      <c r="L35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="C36" s="1">
         <v>18.0</v>
@@ -1404,13 +2062,19 @@
       <c r="H36" s="1">
         <v>1.2</v>
       </c>
+      <c r="L36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C37" s="1">
         <v>16.0</v>
@@ -1430,13 +2094,19 @@
       <c r="H37" s="1">
         <v>1.4</v>
       </c>
+      <c r="L37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="C38" s="1">
         <v>15.0</v>
@@ -1456,29 +2126,62 @@
       <c r="H38" s="1">
         <v>2.1</v>
       </c>
+      <c r="I38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>120</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>85</v>
+        <v>122</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="C41" s="1">
         <v>17.0</v>
@@ -1497,6 +2200,24 @@
       </c>
       <c r="H41" s="1">
         <v>1.9</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1"/>

</xml_diff>